<commit_message>
Week 6 latest Update of TimeLine
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Desktop\CSE110M260T2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Desktop\CSE110M260T2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -375,6 +375,18 @@
   </si>
   <si>
     <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable search for a destination functionality in Gmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Eric Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -382,7 +394,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +449,24 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -545,7 +575,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -612,6 +642,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -648,11 +684,20 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -975,7 +1020,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -984,13 +1029,13 @@
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="36" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="22" t="s">
         <v>86</v>
       </c>
       <c r="G2" s="12" t="s">
@@ -998,14 +1043,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="37" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1019,14 +1064,14 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="36" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1038,33 +1083,33 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>80</v>
+      <c r="D5" s="38" t="s">
+        <v>68</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="23" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="40" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1073,14 +1118,14 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="36" t="s">
         <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1089,14 +1134,14 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="36" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1104,513 +1149,527 @@
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="8" t="s">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
+      <c r="B12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="7" t="s">
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
+      <c r="B13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
+      <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="7" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
+      <c r="B15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="7" t="s">
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="13" t="s">
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C17" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="7" t="s">
+    <row r="19" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="31"/>
+      <c r="B19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="7" t="s">
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
+      <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="8" t="s">
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
+      <c r="B21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="7" t="s">
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
+      <c r="B22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="7" t="s">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="31"/>
+      <c r="B23" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="14" t="s">
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="7" t="s">
+    <row r="26" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="31"/>
+      <c r="B26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G26" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31"/>
+      <c r="B27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G27" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="8" t="s">
+    <row r="28" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G28" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="8" t="s">
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="7" t="s">
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
+      <c r="B30" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G30" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="7" t="s">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="31"/>
+      <c r="B31" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G31" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="G31" s="12" t="s">
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="G32" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
+    <row r="33" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C33" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="F33" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-      <c r="B33" s="8" t="s">
+    <row r="34" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="30"/>
+      <c r="B34" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G34" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
-      <c r="B34" s="21" t="s">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30"/>
+      <c r="B35" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G35" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="28"/>
-      <c r="B35" s="7" t="s">
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="30"/>
+      <c r="B36" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G36" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="28"/>
-      <c r="G36" s="12" t="s">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="30"/>
+      <c r="G37" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="G37" s="12" t="s">
+    <row r="38" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="30"/>
+      <c r="G38" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
-      <c r="G38" s="12" t="s">
+    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="30"/>
+      <c r="G39" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="28"/>
-      <c r="G39" s="12" t="s">
+    <row r="40" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="30"/>
+      <c r="G40" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="28"/>
-      <c r="G40" s="12" t="s">
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="30"/>
+      <c r="G41" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="G41" s="6" t="s">
+    <row r="42" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="35"/>
+      <c r="G42" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B43" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="23"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="23"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="23"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="23"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="23"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="23"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="23"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="23"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-    </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="25"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A42:A51"/>
-    <mergeCell ref="B42:G51"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="B43:G52"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 7 updates of TimeLine
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,10 +170,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Functionality(select bus stop and told when too leave)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Eric Chen, Min Chang Kim</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -362,31 +358,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>User Stories 5 --- Keep Track of User location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable search for a destination functionality in Gmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Eric Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Finished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>In-Progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 5 --- Keep Track of User location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable search for a destination functionality in Gmap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han, Eric Chen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unfinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 9 --- UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(Enter a bus stop number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 4 --- Set alert time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -394,7 +410,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,6 +481,15 @@
       <b/>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -648,6 +673,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -684,19 +721,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1016,11 +1041,11 @@
         <v>2</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1029,29 +1054,29 @@
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>68</v>
+      <c r="D2" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>80</v>
+      <c r="D3" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>23</v>
@@ -1060,19 +1085,19 @@
         <v>19</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>68</v>
+        <v>80</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>24</v>
@@ -1083,34 +1108,34 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>68</v>
+      <c r="D5" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>85</v>
+      <c r="D6" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
@@ -1118,15 +1143,15 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>69</v>
+      <c r="D7" s="24" t="s">
+        <v>68</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
@@ -1134,50 +1159,50 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>68</v>
+      <c r="D8" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="E9" s="7"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>84</v>
+      <c r="D10" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="37" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1186,490 +1211,527 @@
       <c r="C11" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="D11" s="24" t="s">
+        <v>67</v>
+      </c>
       <c r="E11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>37</v>
+      <c r="D12" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>39</v>
+      <c r="D13" s="40" t="s">
+        <v>79</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>41</v>
+      <c r="D14" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="F14" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="G14" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>43</v>
+      <c r="D15" s="40" t="s">
+        <v>79</v>
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
       <c r="B16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="35"/>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="13" t="s">
+      <c r="G19" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="35"/>
+      <c r="B20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="B21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="35"/>
+      <c r="B22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="35"/>
+      <c r="B23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="35"/>
+      <c r="B24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="11" t="s">
+      <c r="F26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-      <c r="B19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="12" t="s">
+    <row r="27" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="35"/>
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
-      <c r="B20" s="7" t="s">
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="35"/>
+      <c r="B28" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="12" t="s">
+      <c r="C28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="12" t="s">
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="35"/>
+      <c r="B29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
-      <c r="B26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
-      <c r="B27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
-      <c r="B28" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="7" t="s">
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="35"/>
+      <c r="B30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="31"/>
-      <c r="B30" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="35"/>
+      <c r="B32" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="G33" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="34"/>
+      <c r="B35" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="G32" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="18" t="s">
+      <c r="C35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="12" t="s">
+      <c r="G35" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="7" t="s">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34"/>
+      <c r="B36" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G36" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="7" t="s">
+    <row r="37" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="34"/>
+      <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G36" s="12" t="s">
+      <c r="C37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="G37" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="34"/>
       <c r="G38" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="34"/>
       <c r="G39" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="30"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="34"/>
       <c r="G40" s="12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
+      <c r="A41" s="34"/>
       <c r="G41" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="34"/>
+      <c r="G42" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="39"/>
+      <c r="G43" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-      <c r="G42" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="25"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="25"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="25"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="25"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="25"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="29"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="30"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="B43:G52"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="B44:G53"/>
     <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A33:A42"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Timeline Week 7
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Desktop\CSE110M260T2\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -386,42 +381,41 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>User Stories 9 --- UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(Enter a bus stop number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 4 --- Set alert time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Unfinished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 9 --- UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality(Enter a bus stop number)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 4 --- Set alert time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -430,7 +424,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -439,14 +433,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -454,7 +448,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -463,7 +457,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -472,7 +466,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -481,7 +475,7 @@
       <b/>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -490,7 +484,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="-0.249977111117893"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -685,6 +679,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -721,12 +718,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -996,7 +990,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1006,22 +1000,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="44.25" customWidth="1"/>
-    <col min="7" max="7" width="34.25" style="17" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="37.5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1044,8 +1038,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A2" s="35" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1067,8 +1061,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A3" s="36"/>
       <c r="B3" s="5" t="s">
         <v>89</v>
       </c>
@@ -1088,8 +1082,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
+    <row r="4" spans="1:7" s="5" customFormat="1">
+      <c r="A4" s="36"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1107,8 +1101,8 @@
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A5" s="36"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1126,8 +1120,8 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
+    <row r="6" spans="1:7" s="5" customFormat="1">
+      <c r="A6" s="36"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1135,15 +1129,15 @@
         <v>17</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
+    <row r="7" spans="1:7" s="5" customFormat="1">
+      <c r="A7" s="36"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1158,8 +1152,8 @@
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
+    <row r="8" spans="1:7" s="5" customFormat="1">
+      <c r="A8" s="36"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1174,8 +1168,8 @@
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A9" s="36"/>
       <c r="B9" s="8" t="s">
         <v>85</v>
       </c>
@@ -1188,8 +1182,8 @@
       <c r="E9" s="7"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A10" s="37"/>
       <c r="B10" s="16" t="s">
         <v>81</v>
       </c>
@@ -1201,8 +1195,8 @@
       </c>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A11" s="38" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1224,10 +1218,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A12" s="36"/>
       <c r="B12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>36</v>
@@ -1239,35 +1233,35 @@
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+    <row r="13" spans="1:7" s="5" customFormat="1">
+      <c r="A13" s="36"/>
       <c r="B13" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="40" t="s">
-        <v>79</v>
+      <c r="D13" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A14" s="36"/>
       <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
@@ -1287,21 +1281,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
+    <row r="15" spans="1:7" s="5" customFormat="1">
+      <c r="A15" s="36"/>
       <c r="B15" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="28" t="s">
         <v>79</v>
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="36"/>
       <c r="B16" s="7" t="s">
         <v>44</v>
       </c>
@@ -1313,8 +1307,8 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A17" s="36"/>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
@@ -1326,21 +1320,21 @@
       </c>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A18" s="37"/>
       <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="40" t="s">
-        <v>79</v>
+      <c r="D18" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A19" s="38" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1359,8 +1353,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
         <v>54</v>
       </c>
@@ -1377,8 +1371,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="35"/>
+    <row r="21" spans="1:7" s="5" customFormat="1">
+      <c r="A21" s="36"/>
       <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
@@ -1395,8 +1389,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A22" s="36"/>
       <c r="B22" s="8" t="s">
         <v>57</v>
       </c>
@@ -1407,8 +1401,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35"/>
+    <row r="23" spans="1:7" s="5" customFormat="1">
+      <c r="A23" s="36"/>
       <c r="B23" s="7" t="s">
         <v>58</v>
       </c>
@@ -1419,8 +1413,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:7" s="5" customFormat="1">
+      <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1429,8 +1423,8 @@
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A25" s="37"/>
       <c r="B25" s="14" t="s">
         <v>61</v>
       </c>
@@ -1439,8 +1433,8 @@
       </c>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
+    <row r="26" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A26" s="38" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -1456,8 +1450,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="35"/>
+    <row r="27" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A27" s="36"/>
       <c r="B27" s="7" t="s">
         <v>39</v>
       </c>
@@ -1471,8 +1465,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
+    <row r="28" spans="1:7" s="5" customFormat="1">
+      <c r="A28" s="36"/>
       <c r="B28" s="7" t="s">
         <v>8</v>
       </c>
@@ -1486,8 +1480,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A29" s="36"/>
       <c r="B29" s="8" t="s">
         <v>63</v>
       </c>
@@ -1498,8 +1492,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A30" s="36"/>
       <c r="B30" s="8" t="s">
         <v>65</v>
       </c>
@@ -1510,8 +1504,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="35"/>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A31" s="36"/>
       <c r="B31" s="7" t="s">
         <v>69</v>
       </c>
@@ -1522,8 +1516,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
+    <row r="32" spans="1:7" s="5" customFormat="1">
+      <c r="A32" s="36"/>
       <c r="B32" s="7" t="s">
         <v>75</v>
       </c>
@@ -1534,14 +1528,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
+    <row r="33" spans="1:7" s="5" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A33" s="37"/>
       <c r="G33" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="38" t="s">
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="30">
+      <c r="A34" s="39" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="18" t="s">
@@ -1557,8 +1551,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A35" s="35"/>
       <c r="B35" s="8" t="s">
         <v>76</v>
       </c>
@@ -1569,8 +1563,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:7" s="5" customFormat="1">
+      <c r="A36" s="35"/>
       <c r="B36" s="21" t="s">
         <v>39</v>
       </c>
@@ -1581,8 +1575,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
+    <row r="37" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A37" s="35"/>
       <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
@@ -1593,135 +1587,135 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
+    <row r="38" spans="1:7" s="5" customFormat="1">
+      <c r="A38" s="35"/>
       <c r="G38" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A39" s="35"/>
       <c r="G39" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
+    <row r="40" spans="1:7" s="5" customFormat="1">
+      <c r="A40" s="35"/>
       <c r="G40" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A41" s="35"/>
       <c r="G41" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A42" s="35"/>
       <c r="G42" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A43" s="40"/>
       <c r="G43" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="28" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="29"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-    </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="30"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="30"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="30"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="30"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="30"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="30"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="30"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="30"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A53" s="31"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Added Additional Week 8 Tasks
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -398,13 +398,22 @@
   </si>
   <si>
     <t>Unfinished</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Fix Google Maps Implementation</t>
+  </si>
+  <si>
+    <t>Min Chang Kim, Eric Chen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +496,14 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -594,7 +611,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -717,6 +734,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -990,7 +1010,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -998,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1343,6 +1363,9 @@
       <c r="C19" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="D19" s="41" t="s">
+        <v>95</v>
+      </c>
       <c r="E19" s="10" t="s">
         <v>23</v>
       </c>
@@ -1416,234 +1439,235 @@
     <row r="24" spans="1:7" s="5" customFormat="1">
       <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" s="5" customFormat="1">
+      <c r="A25" s="36"/>
+      <c r="B25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A25" s="37"/>
-      <c r="B25" s="14" t="s">
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A26" s="37"/>
+      <c r="B26" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C26" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A26" s="38" t="s">
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A27" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A27" s="36"/>
-      <c r="B27" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1">
+    <row r="28" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A28" s="36"/>
       <c r="B28" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="5" customFormat="1">
+      <c r="A29" s="36"/>
+      <c r="B29" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A29" s="36"/>
-      <c r="B29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A30" s="36"/>
       <c r="B30" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A31" s="36"/>
-      <c r="B31" s="7" t="s">
-        <v>69</v>
+      <c r="B31" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A32" s="36"/>
       <c r="B32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1">
+      <c r="A33" s="36"/>
+      <c r="B33" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G33" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A33" s="37"/>
-      <c r="G33" s="12" t="s">
+    <row r="34" spans="1:7" s="5" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A34" s="37"/>
+      <c r="G34" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="19" customFormat="1" ht="30">
-      <c r="A34" s="39" t="s">
+    <row r="35" spans="1:7" s="19" customFormat="1" ht="30">
+      <c r="A35" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B35" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C35" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F35" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A35" s="35"/>
-      <c r="B35" s="8" t="s">
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A36" s="35"/>
+      <c r="B36" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G36" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1">
-      <c r="A36" s="35"/>
-      <c r="B36" s="21" t="s">
+    <row r="37" spans="1:7" s="5" customFormat="1">
+      <c r="A37" s="35"/>
+      <c r="B37" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G37" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A37" s="35"/>
-      <c r="B37" s="7" t="s">
+    <row r="38" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A38" s="35"/>
+      <c r="B38" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G38" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1">
-      <c r="A38" s="35"/>
-      <c r="G38" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="30">
+    <row r="39" spans="1:7" s="5" customFormat="1">
       <c r="A39" s="35"/>
       <c r="G39" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="5" customFormat="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A40" s="35"/>
       <c r="G40" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="30">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="5" customFormat="1">
       <c r="A41" s="35"/>
       <c r="G41" s="12" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A42" s="35"/>
       <c r="G42" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A43" s="35"/>
+      <c r="G43" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A43" s="40"/>
-      <c r="G43" s="6" t="s">
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A44" s="40"/>
+      <c r="G44" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="29" t="s">
+    <row r="45" spans="1:7">
+      <c r="A45" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B45" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="30"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="30"/>
@@ -1708,8 +1732,8 @@
       <c r="F52" s="34"/>
       <c r="G52" s="34"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A53" s="31"/>
+    <row r="53" spans="1:7">
+      <c r="A53" s="30"/>
       <c r="B53" s="34"/>
       <c r="C53" s="34"/>
       <c r="D53" s="34"/>
@@ -1717,15 +1741,24 @@
       <c r="F53" s="34"/>
       <c r="G53" s="34"/>
     </row>
+    <row r="54" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A54" s="31"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="B44:G53"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="B45:G54"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A35:A44"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 8 Update of Timeline
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\刘\Desktop\CSE110M260T2\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,10 +258,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Finish alert functionality</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>User Stories 3 --- Alert actually work</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -265,10 +266,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Capture UCSD shuttle live time ---- Continued working</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Liu Han</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -337,35 +334,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Elyas, Liu Han</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable google maps to keep track of user current location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Chang Kim, Siraj Ghouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 5 --- Keep Track of User location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable search for a destination functionality in Gmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Eric Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 9 --- UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(Enter a bus stop number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 4 --- Set alert time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unfinished</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Fix Google Maps Implementation</t>
+  </si>
+  <si>
+    <t>Min Chang Kim, Eric Chen</t>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unfinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>In-Progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Elyas, Liu Han</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable google maps to keep track of user current location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Min Chang Kim, Siraj Ghouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 5 --- Keep Track of User location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable search for a destination functionality in Gmap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han, Eric Chen</t>
+    <t>In-Progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -373,58 +422,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 9 --- UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality(Enter a bus stop number)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 4 --- Set alert time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unfinished</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
-    <t>Fix Google Maps Implementation</t>
-  </si>
-  <si>
-    <t>Min Chang Kim, Eric Chen</t>
+    <t>Work on UCSD shuttle functionality ---- Continued working</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -433,7 +450,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -442,14 +459,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -457,7 +474,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -466,7 +483,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -475,7 +492,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -484,7 +501,7 @@
       <b/>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -493,7 +510,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -502,7 +519,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -611,7 +636,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -699,6 +724,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -735,12 +763,15 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1010,7 +1041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1018,24 +1049,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="38.375" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="44.25" customWidth="1"/>
+    <col min="7" max="7" width="34.25" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="37.5">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1058,8 +1089,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1069,28 +1100,28 @@
         <v>16</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A3" s="36"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="37"/>
       <c r="B3" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>23</v>
@@ -1099,19 +1130,19 @@
         <v>19</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1">
-      <c r="A4" s="36"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="37"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>24</v>
@@ -1121,8 +1152,8 @@
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A5" s="36"/>
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="37"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1161,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>25</v>
@@ -1140,8 +1171,8 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="37"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1149,15 +1180,15 @@
         <v>17</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1165,15 +1196,15 @@
         <v>12</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1">
-      <c r="A8" s="36"/>
+    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="37"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1181,42 +1212,42 @@
         <v>15</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
       <c r="B9" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E9" s="7"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A10" s="37"/>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
       <c r="B10" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1226,7 +1257,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>23</v>
@@ -1238,29 +1269,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A12" s="36"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
       <c r="B12" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
       <c r="B13" s="7" t="s">
         <v>37</v>
       </c>
@@ -1268,20 +1299,20 @@
         <v>38</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A14" s="36"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
       <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
@@ -1289,7 +1320,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>27</v>
@@ -1301,8 +1332,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1">
-      <c r="A15" s="36"/>
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="37"/>
       <c r="B15" s="7" t="s">
         <v>41</v>
       </c>
@@ -1310,12 +1341,12 @@
         <v>42</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="37"/>
       <c r="B16" s="7" t="s">
         <v>44</v>
       </c>
@@ -1323,12 +1354,12 @@
         <v>45</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="36"/>
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="37"/>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
@@ -1336,12 +1367,12 @@
         <v>7</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A18" s="37"/>
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
       <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
@@ -1349,12 +1380,12 @@
         <v>49</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A19" s="38" t="s">
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1363,8 +1394,8 @@
       <c r="C19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="41" t="s">
-        <v>95</v>
+      <c r="D19" s="29" t="s">
+        <v>92</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>23</v>
@@ -1376,32 +1407,38 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="37"/>
       <c r="B20" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="D20" s="42" t="s">
+        <v>95</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="37"/>
       <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="D21" s="43" t="s">
+        <v>98</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
@@ -1412,109 +1449,121 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="37"/>
       <c r="B22" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="D22" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="G22" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="37"/>
       <c r="B23" s="7" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="5" customFormat="1">
-      <c r="A24" s="36"/>
+        <v>94</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="37"/>
       <c r="B24" s="7" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>97</v>
+        <v>45</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>95</v>
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1">
-      <c r="A25" s="36"/>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="37"/>
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A26" s="37"/>
-      <c r="B26" s="14" t="s">
+      <c r="F27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="37"/>
+      <c r="B28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="37"/>
+      <c r="B29" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A27" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A28" s="36"/>
-      <c r="B28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1">
-      <c r="A29" s="36"/>
-      <c r="B29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="G29" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A30" s="36"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="37"/>
       <c r="B30" s="8" t="s">
         <v>63</v>
       </c>
@@ -1522,243 +1571,231 @@
         <v>64</v>
       </c>
       <c r="G30" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="37"/>
+      <c r="B31" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="37"/>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="38"/>
+      <c r="G33" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="36"/>
+      <c r="B35" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="36"/>
+      <c r="B36" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="36"/>
+      <c r="B37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A31" s="36"/>
-      <c r="B31" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="12" t="s">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="36"/>
+      <c r="G38" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A32" s="36"/>
-      <c r="B32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="7" t="s">
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="36"/>
+      <c r="G39" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="36"/>
+      <c r="G40" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="36"/>
+      <c r="G41" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="36"/>
+      <c r="G42" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="5" customFormat="1">
-      <c r="A33" s="36"/>
-      <c r="B33" s="7" t="s">
+    </row>
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="41"/>
+      <c r="G43" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A34" s="37"/>
-      <c r="G34" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="19" customFormat="1" ht="30">
-      <c r="A35" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A36" s="35"/>
-      <c r="B36" s="8" t="s">
+      <c r="B44" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="5" customFormat="1">
-      <c r="A37" s="35"/>
-      <c r="B37" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A38" s="35"/>
-      <c r="B38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="5" customFormat="1">
-      <c r="A39" s="35"/>
-      <c r="G39" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A40" s="35"/>
-      <c r="G40" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="5" customFormat="1">
-      <c r="A41" s="35"/>
-      <c r="G41" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A42" s="35"/>
-      <c r="G42" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" ht="30">
-      <c r="A43" s="35"/>
-      <c r="G43" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A44" s="40"/>
-      <c r="G44" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="30"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="30"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="30"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="30"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="30"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="30"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="30"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="30"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A54" s="31"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="31"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="31"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="31"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="31"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="31"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="31"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="31"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="31"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="32"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="B45:G54"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="B44:G53"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Final Week Tasks
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Desktop\CSE110M260T2\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,10 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Week 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Feedback from clients</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -322,126 +313,128 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>At the End of Week 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deliver Final APP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elyas, Liu Han</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable google maps to keep track of user current location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Chang Kim, Siraj Ghouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 5 --- Keep Track of User location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable search for a destination functionality in Gmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Eric Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 9 --- UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(Enter a bus stop number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 4 --- Set alert time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unfinished</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Fix Google Maps Implementation</t>
+  </si>
+  <si>
+    <t>Min Chang Kim, Eric Chen</t>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unfinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In-Progress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In-Progress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work on UCSD shuttle functionality ---- Continued working</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">Enable functionality of getting waiting time of line </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>At the End of Week 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deliver Final APP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elyas, Liu Han</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable google maps to keep track of user current location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Min Chang Kim, Siraj Ghouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 5 --- Keep Track of User location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable search for a destination functionality in Gmap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han, Eric Chen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 9 --- UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality(Enter a bus stop number)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 4 --- Set alert time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unfinished</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
-    <t>Fix Google Maps Implementation</t>
-  </si>
-  <si>
-    <t>Min Chang Kim, Eric Chen</t>
-  </si>
-  <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unfinished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In-Progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In-Progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work on UCSD shuttle functionality ---- Continued working</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Members</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -450,7 +443,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -459,14 +452,7 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -474,7 +460,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -483,7 +469,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -492,7 +478,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -501,7 +487,7 @@
       <b/>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -510,7 +496,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="-0.249977111117893"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -519,7 +505,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -527,7 +513,7 @@
       <b/>
       <sz val="11"/>
       <color theme="4"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -636,7 +622,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -691,55 +677,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -751,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,18 +737,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1041,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1049,24 +1020,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.375" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="44.25" customWidth="1"/>
-    <col min="7" max="7" width="34.25" style="17" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="37.5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1086,11 +1057,11 @@
         <v>2</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A2" s="35" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1099,29 +1070,29 @@
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>65</v>
+      <c r="D2" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>80</v>
+      <c r="F2" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A3" s="36"/>
       <c r="B3" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>85</v>
+      <c r="D3" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>23</v>
@@ -1130,19 +1101,19 @@
         <v>19</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1">
+      <c r="A4" s="36"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>24</v>
@@ -1152,650 +1123,612 @@
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A5" s="36"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>65</v>
+      <c r="D5" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>51</v>
+      <c r="F5" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:7" s="5" customFormat="1">
+      <c r="A6" s="36"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>91</v>
+      <c r="D6" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
+    <row r="7" spans="1:7" s="5" customFormat="1">
+      <c r="A7" s="36"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>66</v>
+      <c r="D7" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+    <row r="8" spans="1:7" s="5" customFormat="1">
+      <c r="A8" s="36"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>65</v>
+      <c r="D8" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A9" s="36"/>
       <c r="B9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>84</v>
       </c>
       <c r="E9" s="7"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A10" s="37"/>
       <c r="B10" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>85</v>
+        <v>77</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>35</v>
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A11" s="38" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>65</v>
+      <c r="D11" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A12" s="36"/>
       <c r="B12" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>85</v>
+        <v>35</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+    <row r="13" spans="1:7" s="5" customFormat="1">
+      <c r="A13" s="36"/>
       <c r="B13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>91</v>
+      <c r="D13" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A14" s="36"/>
       <c r="B14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>65</v>
+      <c r="D14" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+    <row r="15" spans="1:7" s="5" customFormat="1">
+      <c r="A15" s="36"/>
       <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>96</v>
+      <c r="D15" s="25" t="s">
+        <v>94</v>
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="36"/>
       <c r="B16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>65</v>
+      <c r="D16" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A17" s="36"/>
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>85</v>
+      <c r="D17" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A18" s="37"/>
       <c r="B18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>91</v>
+      <c r="D18" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="41" t="s">
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A19" s="38" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>92</v>
+        <v>33</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>95</v>
+      <c r="D20" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="39"/>
+    <row r="21" spans="1:7" s="5" customFormat="1">
+      <c r="A21" s="36"/>
       <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>96</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A22" s="36"/>
       <c r="B22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>97</v>
+        <v>35</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>95</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
+    <row r="23" spans="1:7" s="5" customFormat="1">
+      <c r="A23" s="36"/>
       <c r="B23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>95</v>
-      </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
+    <row r="24" spans="1:7" s="5" customFormat="1">
+      <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>95</v>
+        <v>44</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>93</v>
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A25" s="37"/>
       <c r="B25" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>99</v>
+        <v>48</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>97</v>
       </c>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="41" t="s">
+    <row r="26" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="A26" s="38" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>34</v>
+      <c r="D26" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
+    <row r="27" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A27" s="36"/>
       <c r="B27" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
+    <row r="28" spans="1:7" s="5" customFormat="1">
+      <c r="A28" s="36"/>
       <c r="B28" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="D28" s="22" t="s">
+        <v>90</v>
+      </c>
       <c r="F28" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A29" s="36"/>
       <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A30" s="36"/>
       <c r="B30" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="G30" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="30">
+      <c r="A31" s="36"/>
       <c r="B31" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="G31" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1">
+      <c r="A32" s="36"/>
+      <c r="B32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="7" t="s">
+      <c r="G32" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="5" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A33" s="37"/>
+      <c r="B33" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="18" customFormat="1">
+      <c r="A34" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
-      <c r="G33" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="B35" s="8" t="s">
+      <c r="B34" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="38"/>
-      <c r="B36" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="38"/>
-      <c r="B37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="38"/>
-      <c r="G38" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="38"/>
-      <c r="G39" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="38"/>
-      <c r="G40" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="38"/>
-      <c r="G41" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="38"/>
-      <c r="G42" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
-      <c r="G43" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="33"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="33"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="33"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="33"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="33"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="33"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="33"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="33"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-    </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="1:11" s="5" customFormat="1">
+      <c r="A35" s="30"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="1:11" s="5" customFormat="1">
+      <c r="A36" s="30"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="1:11" s="5" customFormat="1">
+      <c r="A37" s="30"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="1:11" s="5" customFormat="1">
+      <c r="A38" s="30"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="1:11" s="5" customFormat="1">
+      <c r="A39" s="30"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="1:11" s="5" customFormat="1">
+      <c r="A40" s="30"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="1:11" s="5" customFormat="1">
+      <c r="A41" s="30"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="1:11" s="5" customFormat="1">
+      <c r="A42" s="30"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="1:11" s="6" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A43" s="31"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="B44:G53"/>
+  <mergeCells count="6">
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:G43"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated User Stories and Timeline
</commit_message>
<xml_diff>
--- a/Documents/TimeLine.xlsx
+++ b/Documents/TimeLine.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,147 +205,187 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Capture UCSD shuttle live time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Siraj Ghouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished User Stories(IDEALLY)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feedback from clients</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update User Stories and Timeline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siraj Ghouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(select bus stop and told when too leave) ---- Continued working</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 3 --- Alert actually work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test and merge codes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine all functionality of MTS ans SD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elyas,ChengYuan Cheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(Input a destination and be told when to leave)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChengYuan Cheng, Eric Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capture live feeds for buses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Min Chang Kim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 2 --- Input a destination and be told when to leave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 7 --- Capture live feeds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>At the End of Week 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deliver Final APP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elyas, Liu Han</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable google maps to keep track of user current location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Chang Kim, Siraj Ghouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 5 --- Keep Track of User location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable search for a destination functionality in Gmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liu Han, Eric Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 9 --- UI Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functionality(Enter a bus stop number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>User Stories 4 --- Set alert time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Capture UCSD shuttle live time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han, Siraj Ghouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished User Stories(IDEALLY)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Feedback from clients</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update User Stories and Timeline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Siraj Ghouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality(select bus stop and told when too leave) ---- Continued working</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 3 --- Alert actually work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test and merge codes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine all functionality of MTS ans SD shuttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elyas,ChengYuan Cheng</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality(Input a destination and be told when to leave)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChengYuan Cheng, Eric Chen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Unfinished</t>
   </si>
   <si>
     <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fix Google Maps Implementation</t>
+  </si>
+  <si>
+    <t>Min Chang Kim, Eric Chen</t>
   </si>
   <si>
     <t>Finished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Capture live feeds for buses</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han, Min Chang Kim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elyas, Siraj Ghouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 2 --- Input a destination and be told when to leave</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 7 --- Capture live feeds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 8 ---- Waiting time of line at bus stop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Figure out how to get waiting time of line</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>At the End of Week 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deliver Final APP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elyas, Liu Han</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable google maps to keep track of user current location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Min Chang Kim, Siraj Ghouse</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 5 --- Keep Track of User location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 10 --- Separate the MTS and SD shuttle Activities pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable search for a destination functionality in Gmap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu Han, Eric Chen</t>
+    <t>Unfinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In-Progress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In-Progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -353,70 +393,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 9 --- UI Design</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality(Enter a bus stop number)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 11 --- Capture live time of UCSD shuttle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Stories 4 --- Set alert time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unfinished</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
-    <t>Fix Google Maps Implementation</t>
-  </si>
-  <si>
-    <t>Min Chang Kim, Eric Chen</t>
-  </si>
-  <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unfinished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In-Progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In-Progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Work on UCSD shuttle functionality ---- Continued working</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable functionality of getting waiting time of line </t>
-  </si>
-  <si>
-    <t>All Members</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +990,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1022,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1057,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="30">
@@ -1071,28 +1049,28 @@
         <v>16</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A3" s="36"/>
       <c r="B3" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>23</v>
@@ -1101,7 +1079,7 @@
         <v>19</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1">
@@ -1110,10 +1088,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>24</v>
@@ -1132,13 +1110,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="12"/>
     </row>
@@ -1151,7 +1129,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
@@ -1167,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
@@ -1183,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>42</v>
@@ -1193,13 +1171,13 @@
     <row r="9" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A9" s="36"/>
       <c r="B9" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E9" s="7"/>
       <c r="G9" s="12"/>
@@ -1207,13 +1185,13 @@
     <row r="10" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
       <c r="A10" s="37"/>
       <c r="B10" s="16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G10" s="16"/>
     </row>
@@ -1228,7 +1206,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>23</v>
@@ -1243,19 +1221,19 @@
     <row r="12" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A12" s="36"/>
       <c r="B12" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>19</v>
@@ -1270,16 +1248,16 @@
         <v>37</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="30">
@@ -1291,7 +1269,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>27</v>
@@ -1312,7 +1290,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G15" s="12"/>
     </row>
@@ -1325,7 +1303,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="12"/>
     </row>
@@ -1338,20 +1316,20 @@
         <v>7</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1">
       <c r="A18" s="37"/>
       <c r="B18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="D18" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G18" s="16"/>
     </row>
@@ -1360,13 +1338,13 @@
         <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>23</v>
@@ -1381,19 +1359,19 @@
     <row r="20" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="D20" s="27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>19</v>
@@ -1405,16 +1383,16 @@
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>20</v>
@@ -1423,13 +1401,13 @@
     <row r="22" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A22" s="36"/>
       <c r="B22" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>28</v>
@@ -1438,39 +1416,39 @@
     <row r="23" spans="1:7" s="5" customFormat="1">
       <c r="A23" s="36"/>
       <c r="B23" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" s="5" customFormat="1">
       <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" s="6" customFormat="1" ht="30.75" thickBot="1">
       <c r="A25" s="37"/>
       <c r="B25" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G25" s="16"/>
     </row>
@@ -1485,10 +1463,10 @@
         <v>33</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>18</v>
@@ -1500,10 +1478,10 @@
         <v>38</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>19</v>
@@ -1518,10 +1496,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>20</v>
@@ -1530,10 +1505,10 @@
     <row r="29" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A29" s="36"/>
       <c r="B29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>28</v>
@@ -1542,22 +1517,20 @@
     <row r="30" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A30" s="36"/>
       <c r="B30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" s="5" customFormat="1" ht="30">
       <c r="A31" s="36"/>
       <c r="B31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>45</v>
@@ -1565,34 +1538,26 @@
     </row>
     <row r="32" spans="1:7" s="5" customFormat="1">
       <c r="A32" s="36"/>
-      <c r="B32" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="G32" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="5" customFormat="1" ht="30.75" thickBot="1">
       <c r="A33" s="37"/>
-      <c r="B33" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>100</v>
-      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="7"/>
       <c r="G33" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="18" customFormat="1">
       <c r="A34" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>

</xml_diff>